<commit_message>
Some Modification on the English sentences
</commit_message>
<xml_diff>
--- a/CRS&SRS&SIQ&RTM/CRS&SRS&SIQ&RTM.xlsx
+++ b/CRS&SRS&SIQ&RTM/CRS&SRS&SIQ&RTM.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="CRS" sheetId="2" r:id="rId1"/>
+    <sheet name="CRS" sheetId="6" r:id="rId1"/>
     <sheet name="SRS" sheetId="3" r:id="rId2"/>
     <sheet name="SIQ" sheetId="5" r:id="rId3"/>
     <sheet name="RTM" sheetId="4" r:id="rId4"/>
@@ -133,9 +133,6 @@
     <t>CRS_00_6, CRS_00_10, CRS_00_11, CRS_00_12, CRS_00_13, CRS_00_14</t>
   </si>
   <si>
-    <t>Read the temperature from the  air.</t>
-  </si>
-  <si>
     <t>Three speed levels for the fan system.</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>SIQ FOR FAN CONTROLLER SYSTEM</t>
+  </si>
+  <si>
+    <t>Read the air temperature.</t>
   </si>
 </sst>
 </file>
@@ -492,383 +492,6 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -935,6 +558,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -964,13 +594,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -982,6 +605,383 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -997,52 +997,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B16" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
   <autoFilter ref="A2:B16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" name=" Description" dataDxfId="21"/>
+    <tableColumn id="1" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" name=" Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B8" totalsRowShown="0" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B8" totalsRowShown="0" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A2:B8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" name=" Description" dataDxfId="15"/>
+    <tableColumn id="1" name="ID" dataDxfId="23"/>
+    <tableColumn id="2" name=" Description" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:F9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:F9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A2:F9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Requirements  ID" dataDxfId="12"/>
-    <tableColumn id="2" name="Questionnaire" dataDxfId="11"/>
-    <tableColumn id="3" name="Customer  Answer" dataDxfId="10"/>
-    <tableColumn id="4" name="From" dataDxfId="9"/>
-    <tableColumn id="5" name="To" dataDxfId="8"/>
-    <tableColumn id="6" name="Date" dataDxfId="7"/>
+    <tableColumn id="1" name="Requirements  ID" dataDxfId="19"/>
+    <tableColumn id="2" name="Questionnaire" dataDxfId="18"/>
+    <tableColumn id="3" name="Customer  Answer" dataDxfId="17"/>
+    <tableColumn id="4" name="From" dataDxfId="16"/>
+    <tableColumn id="5" name="To" dataDxfId="15"/>
+    <tableColumn id="6" name="Date" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A2:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="CRS" dataDxfId="5"/>
-    <tableColumn id="2" name="SRS" dataDxfId="4"/>
-    <tableColumn id="3" name="DESIGN" dataDxfId="3"/>
-    <tableColumn id="4" name="CODE" dataDxfId="2"/>
-    <tableColumn id="5" name="TEST" dataDxfId="1"/>
-    <tableColumn id="6" name="RELATED SRS" dataDxfId="0"/>
+    <tableColumn id="1" name="CRS" dataDxfId="12"/>
+    <tableColumn id="2" name="SRS" dataDxfId="11"/>
+    <tableColumn id="3" name="DESIGN" dataDxfId="10"/>
+    <tableColumn id="4" name="CODE" dataDxfId="9"/>
+    <tableColumn id="5" name="TEST" dataDxfId="8"/>
+    <tableColumn id="6" name="RELATED SRS" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1338,7 +1338,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="1"/>
@@ -1367,7 +1367,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1455,7 +1455,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1463,7 +1463,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1491,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1505,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="22"/>
     </row>
@@ -1562,7 +1562,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1597,7 +1597,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1607,39 +1607,39 @@
     </row>
     <row r="2" spans="1:6" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>75</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="F3" s="19">
         <v>42717</v>
@@ -1647,19 +1647,19 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>59</v>
-      </c>
       <c r="D4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="F4" s="19">
         <v>42717</v>
@@ -1667,19 +1667,19 @@
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="C5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>63</v>
-      </c>
       <c r="E5" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="19">
         <v>42717</v>
@@ -1687,19 +1687,19 @@
     </row>
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>65</v>
-      </c>
       <c r="C6" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="19">
         <v>42717</v>
@@ -1707,19 +1707,19 @@
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="F7" s="19">
         <v>42717</v>
@@ -1727,19 +1727,19 @@
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>71</v>
-      </c>
       <c r="D8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="F8" s="19">
         <v>42717</v>
@@ -1747,19 +1747,19 @@
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>73</v>
-      </c>
       <c r="C9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="F9" s="19">
         <v>42717</v>
@@ -1796,7 +1796,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>

</xml_diff>

<commit_message>
Just Separate the SIQ
</commit_message>
<xml_diff>
--- a/CRS&SRS&SIQ&RTM/CRS&SRS&SIQ&RTM.xlsx
+++ b/CRS&SRS&SIQ&RTM/CRS&SRS&SIQ&RTM.xlsx
@@ -9,14 +9,13 @@
   <sheets>
     <sheet name="CRS" sheetId="6" r:id="rId1"/>
     <sheet name="SRS" sheetId="3" r:id="rId2"/>
-    <sheet name="SIQ" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -145,97 +144,10 @@
     <t>Design a PCB for the battery powered system with a switch for the power controlling</t>
   </si>
   <si>
-    <t>Requirements  ID</t>
-  </si>
-  <si>
-    <t>CR_00_5</t>
-  </si>
-  <si>
-    <t>Do you want  to make the fan's speed levels  configurable  or not ?</t>
-  </si>
-  <si>
-    <t>yes  , I  want</t>
-  </si>
-  <si>
-    <t>Yasser</t>
-  </si>
-  <si>
-    <t>Eng/Waleed</t>
-  </si>
-  <si>
-    <t>CR_00_8</t>
-  </si>
-  <si>
-    <t>DO  you want   moving or static  displaying ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">static  displaying </t>
-  </si>
-  <si>
-    <t>CR_00_9</t>
-  </si>
-  <si>
-    <t>What is the initial displaying state  of the LCD?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nothing  Iwant it initially  empty </t>
-  </si>
-  <si>
-    <t>Mariam</t>
-  </si>
-  <si>
-    <t>CR_00_6</t>
-  </si>
-  <si>
-    <t>Do you want a switch  for  powering  system?</t>
-  </si>
-  <si>
-    <t>CR_00_12</t>
-  </si>
-  <si>
-    <t>What is the final  shape of the system?</t>
-  </si>
-  <si>
-    <t>I want the  system to be on a PCB.</t>
-  </si>
-  <si>
-    <t>CR_00_13</t>
-  </si>
-  <si>
-    <t>is there any constrains on the size of the board?</t>
-  </si>
-  <si>
-    <t>yes, I want it  small  as much as you can .</t>
-  </si>
-  <si>
-    <t>CR_00_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you want to  make the system portable  by using  battery? </t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer  Answer</t>
-  </si>
-  <si>
-    <t>Questionnaire</t>
-  </si>
-  <si>
     <t>SRS FOR FAN CONTROLLER SYSTEM</t>
   </si>
   <si>
     <t>CRS FOR FAN CONTROLLER SYSTEM</t>
-  </si>
-  <si>
-    <t>SIQ FOR FAN CONTROLLER SYSTEM</t>
   </si>
   <si>
     <t>Read the air temperature.</t>
@@ -367,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -403,143 +315,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <strike val="0"/>
@@ -764,37 +550,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A2:B16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ID" dataDxfId="15"/>
-    <tableColumn id="2" name=" Description" dataDxfId="14"/>
+    <tableColumn id="1" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" name=" Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B8" totalsRowShown="0" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B8" totalsRowShown="0" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A2:B8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ID" dataDxfId="9"/>
-    <tableColumn id="2" name=" Description" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:F9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F9"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Requirements  ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Questionnaire" dataDxfId="4"/>
-    <tableColumn id="3" name="Customer  Answer" dataDxfId="3"/>
-    <tableColumn id="4" name="From" dataDxfId="2"/>
-    <tableColumn id="5" name="To" dataDxfId="1"/>
-    <tableColumn id="6" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" name=" Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1100,10 +871,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="13"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1119,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1256,10 +1027,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1327,203 +1098,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="14">
-        <v>42717</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>